<commit_message>
coder thanh son has added data id 12
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimhu\OneDrive\Máy tính\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\php\androi-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30823C55-E1F1-4044-873C-D7F17B05E86E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{8A41AC7B-F4E5-40C1-9EDA-9B9C3CCDCF06}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TaiKhoan" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="ChuDe" sheetId="4" r:id="rId4"/>
     <sheet name="MonAn" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -453,12 +452,32 @@
   <si>
     <t>status_MA</t>
   </si>
+  <si>
+    <t>Dưa góp đu đủ cà rốt</t>
+  </si>
+  <si>
+    <t>1 quả đu đủ
+1 củ cà rốt
+4 tép tỏi
+1 quả ớt băm nhỏ
+Nước mắm
+Gia vị khác</t>
+  </si>
+  <si>
+    <t>Đu đủ nạo vỏ, hạt trong ruột, ngâm nước cho ra hết nhựa.Cà rốt rửa sạch, thái lát mỏng, vừa ăn</t>
+  </si>
+  <si>
+    <t>Món dưa góp muối nước mắm này để khoảng 1 ngày là ăn được, có thể để cỡ 1 tuần nếu cho vào ngăn mát tủ lạnh.</t>
+  </si>
+  <si>
+    <t>Cho 2 thìa nhỏ muối và 2 thìa canh đường vào bát sau đó trộn đều để ngấm.Đu đủ, cà rốt, dưa chuột trộn đều rồi cho vào hũ thủy tinh đã tiệt trùng  rồi chế nước ngâm vào sao cho ngập hỗn hợp nguyên liệu. Nhớ gài que tre hay bát đĩa để đu đủ, cà rốt, dưa chuột không nổi lên rồi đậy kín hũ. Để hủ nơi thoáng mát.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,6 +492,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -496,7 +522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -519,6 +545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -833,7 +860,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285B6299-AAB3-4EE5-ABA4-24D8274220B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -923,7 +950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFC0272-A337-4791-9190-AFE9C2F2A484}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -999,7 +1026,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE150D70-3B77-4E5D-96B4-8D0DB8A1E3EB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1066,14 +1093,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{ED6DBA45-20EC-4F10-A38A-FA10C76E2411}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555D946F-C718-41A0-A976-3F80A480DBAF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1115,12 +1142,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED20FD39-F807-4741-AA9C-580341BA5154}">
-  <dimension ref="A1:J12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1422,7 +1449,31 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="J13" s="6">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
xong giao dien đăng nhập, đăng ký
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimhu\OneDrive\Máy tính\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK5\android\androi-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7633C8-5CF3-46B2-8969-B926DDF382A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0A7025-1D18-469A-B463-6DCB811F3AE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{8A41AC7B-F4E5-40C1-9EDA-9B9C3CCDCF06}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{8A41AC7B-F4E5-40C1-9EDA-9B9C3CCDCF06}"/>
   </bookViews>
   <sheets>
     <sheet name="TaiKhoan" sheetId="1" r:id="rId1"/>
@@ -1544,16 +1544,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE150D70-3B77-4E5D-96B4-8D0DB8A1E3EB}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1660,7 +1660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED20FD39-F807-4741-AA9C-580341BA5154}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
     </sheetView>

</xml_diff>